<commit_message>
added basic data type error
</commit_message>
<xml_diff>
--- a/Project/Testing/Excel_File.xlsx
+++ b/Project/Testing/Excel_File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36140F69-F275-4CEF-846E-40DB4517328F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6618C72-2995-4F02-ABF6-2C7F61DB87C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3600" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="4635" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Dillon</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Int_test</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>dfe</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
   <dimension ref="B4:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +417,9 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -422,7 +433,9 @@
       <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -437,6 +450,9 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
@@ -447,6 +463,9 @@
       </c>
       <c r="F7" t="s">
         <v>5</v>
+      </c>
+      <c r="G7">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>